<commit_message>
Fix formatting and clean code a bit
</commit_message>
<xml_diff>
--- a/hello.xlsx
+++ b/hello.xlsx
@@ -17,13 +17,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
+    <t>Chart Title</t>
+  </si>
+  <si>
     <t>Dial Colors</t>
   </si>
   <si>
     <t>Needle</t>
-  </si>
-  <si>
-    <t>Chart Title</t>
   </si>
 </sst>
 </file>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"><c:lang val="en-US"/><c:chart><c:plotArea><c:layout/><c:doughnutChart><c:varyColors val="1"/><c:ser><c:idx val="0"/><c:order val="0"/><c:dPt><c:idx val="0"/><c:spPr><a:solidFill><a:srgbClr val="FC7613"/></a:solidFill></c:spPr></c:dPt><c:dPt><c:idx val="1"/><c:spPr><a:solidFill><a:srgbClr val="FFD641"/></a:solidFill></c:spPr></c:dPt><c:dPt><c:idx val="2"/><c:spPr><a:solidFill><a:srgbClr val="B6C94C"/></a:solidFill></c:spPr></c:dPt><c:dPt><c:idx val="3"/><c:spPr><a:noFill/></c:spPr></c:dPt><c:dPt><c:idx val="4"/><c:spPr><a:noFill/></c:spPr></c:dPt><c:dPt><c:idx val="5"/><c:spPr><a:noFill/></c:spPr></c:dPt><c:val><c:numRef><c:f>Sheet1!$A2:$A$7</c:f><c:numCache><c:formatCode>General</c:formatCode><c:ptCount val="6"/><c:pt idx="0"><c:v>60</c:v></c:pt><c:pt idx="1"><c:v>60</c:v></c:pt><c:pt idx="2"><c:v>60</c:v></c:pt><c:pt idx="3"><c:v>60</c:v></c:pt><c:pt idx="4"><c:v>60</c:v></c:pt><c:pt idx="5"><c:v>60</c:v></c:pt></c:numCache></c:numRef></c:val></c:ser><c:firstSliceAng val="270"/></c:doughChart></c:plotArea><c:legend><c:legendPos val="r"/><c:layout/><c:txPr><a:bodyPr/><a:lstStyle/><a:p><a:pPr rtl="0"><a:defRPr/></a:pPr><a:endParaRPr lang="en-US"/></a:p></c:txPr></c:legend><c:plotVisOnly val="1"/></c:chart><c:printSettings><c:headerFooter/><c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/><c:pageSetup/></c:printSettings></c:chartSpace>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"><c:lang val="en-US"/><c:chart><c:plotArea><c:layout/><c:doughnutChart><c:varyColors val="1"/><c:ser><c:idx val="0"/><c:order val="0"/><c:dPt><c:idx val="0"/><c:spPr><a:solidFill><a:srgbClr val="FC7613"/></a:solidFill></c:spPr></c:dPt><c:dPt><c:idx val="1"/><c:spPr><a:solidFill><a:srgbClr val="FFD641"/></a:solidFill></c:spPr></c:dPt><c:dPt><c:idx val="2"/><c:spPr><a:solidFill><a:srgbClr val="B6C94C"/></a:solidFill></c:spPr></c:dPt><c:dPt><c:idx val="3"/><c:spPr><a:noFill/></c:spPr></c:dPt><c:dPt><c:idx val="4"/><c:spPr><a:noFill/></c:spPr></c:dPt><c:dPt><c:idx val="5"/><c:spPr><a:noFill/></c:spPr></c:dPt><c:val><c:numRef><c:f>Sheet2!$A2:$A$7</c:f><c:numCache><c:formatCode>General</c:formatCode><c:ptCount val="6"/><c:pt idx="0"><c:v>60</c:v></c:pt><c:pt idx="1"><c:v>60</c:v></c:pt><c:pt idx="2"><c:v>60</c:v></c:pt><c:pt idx="3"><c:v>60</c:v></c:pt><c:pt idx="4"><c:v>60</c:v></c:pt><c:pt idx="5"><c:v>60</c:v></c:pt></c:numCache></c:numRef></c:val></c:ser><c:firstSliceAng val="270"/></c:doughChart></c:plotArea><c:legend><c:legendPos val="r"/><c:layout/><c:txPr><a:bodyPr/><a:lstStyle/><a:p><a:pPr rtl="0"><a:defRPr/></a:pPr><a:endParaRPr lang="en-US"/></a:p></c:txPr></c:legend><c:plotVisOnly val="1"/></c:chart><c:printSettings><c:headerFooter/><c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/><c:pageSetup/></c:printSettings></c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2285,15 +2285,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2315,15 +2315,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>-95249</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2631,72 +2631,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2">
-        <v>60</v>
-      </c>
-      <c r="B2">
-        <v>180</v>
-      </c>
-      <c r="C2">
-        <f>$C$3 &amp; "% Share"</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <f>$A$3 &amp; "% Share"</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3">
-        <v>60</v>
-      </c>
-      <c r="B3">
-        <f>((180/200)*(C3+100))-B4</f>
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>60</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>60</v>
-      </c>
-      <c r="B5">
-        <f>360-SUM(B2:B4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2707,144 +2661,184 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D2:E361"/>
+  <dimension ref="A1:E361"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="4:5">
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>60</v>
+      </c>
+      <c r="B2">
+        <v>180</v>
+      </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="4:5">
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>60</v>
+      </c>
+      <c r="B3">
+        <f>((180/200)*(Sheet1!A3+100))-B4</f>
+        <v>0</v>
+      </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="4:5">
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>60</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="4:5">
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>60</v>
+      </c>
+      <c r="B5">
+        <f>360-SUM(B2:B4)</f>
+        <v>0</v>
+      </c>
       <c r="D5">
         <v>3</v>
       </c>
       <c r="E5">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="4:5">
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>60</v>
+      </c>
       <c r="D6">
         <v>4</v>
       </c>
       <c r="E6">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="4:5">
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>60</v>
+      </c>
       <c r="D7">
         <v>5</v>
       </c>
       <c r="E7">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="4:5">
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="D8">
         <v>6</v>
       </c>
       <c r="E8">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="4:5">
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="D9">
         <v>7</v>
       </c>
       <c r="E9">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="4:5">
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="D10">
         <v>8</v>
       </c>
       <c r="E10">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="4:5">
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="D11">
         <v>9</v>
       </c>
       <c r="E11">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="4:5">
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="D12">
         <v>10</v>
       </c>
       <c r="E12">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="4:5">
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="D13">
         <v>11</v>
       </c>
       <c r="E13">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="4:5">
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="D14">
         <v>12</v>
       </c>
       <c r="E14">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="4:5">
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="D15">
         <v>13</v>
       </c>
       <c r="E15">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="4:5">
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="D16">
         <v>14</v>
       </c>
       <c r="E16">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2853,7 +2847,7 @@
         <v>15</v>
       </c>
       <c r="E17">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2862,7 +2856,7 @@
         <v>16</v>
       </c>
       <c r="E18">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2871,7 +2865,7 @@
         <v>17</v>
       </c>
       <c r="E19">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2880,7 +2874,7 @@
         <v>18</v>
       </c>
       <c r="E20">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2889,7 +2883,7 @@
         <v>19</v>
       </c>
       <c r="E21">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2898,7 +2892,7 @@
         <v>20</v>
       </c>
       <c r="E22">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2907,7 +2901,7 @@
         <v>21</v>
       </c>
       <c r="E23">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2916,7 +2910,7 @@
         <v>22</v>
       </c>
       <c r="E24">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2925,7 +2919,7 @@
         <v>23</v>
       </c>
       <c r="E25">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2934,7 +2928,7 @@
         <v>24</v>
       </c>
       <c r="E26">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2943,7 +2937,7 @@
         <v>25</v>
       </c>
       <c r="E27">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2952,7 +2946,7 @@
         <v>26</v>
       </c>
       <c r="E28">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2961,7 +2955,7 @@
         <v>27</v>
       </c>
       <c r="E29">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2970,7 +2964,7 @@
         <v>28</v>
       </c>
       <c r="E30">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2979,7 +2973,7 @@
         <v>29</v>
       </c>
       <c r="E31">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2988,7 +2982,7 @@
         <v>30</v>
       </c>
       <c r="E32">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2997,7 +2991,7 @@
         <v>31</v>
       </c>
       <c r="E33">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3006,7 +3000,7 @@
         <v>32</v>
       </c>
       <c r="E34">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3015,7 +3009,7 @@
         <v>33</v>
       </c>
       <c r="E35">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3024,7 +3018,7 @@
         <v>34</v>
       </c>
       <c r="E36">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3033,7 +3027,7 @@
         <v>35</v>
       </c>
       <c r="E37">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3042,7 +3036,7 @@
         <v>36</v>
       </c>
       <c r="E38">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3051,7 +3045,7 @@
         <v>37</v>
       </c>
       <c r="E39">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3060,7 +3054,7 @@
         <v>38</v>
       </c>
       <c r="E40">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3069,7 +3063,7 @@
         <v>39</v>
       </c>
       <c r="E41">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3078,7 +3072,7 @@
         <v>40</v>
       </c>
       <c r="E42">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3087,7 +3081,7 @@
         <v>41</v>
       </c>
       <c r="E43">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3096,7 +3090,7 @@
         <v>42</v>
       </c>
       <c r="E44">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3105,7 +3099,7 @@
         <v>43</v>
       </c>
       <c r="E45">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3114,7 +3108,7 @@
         <v>44</v>
       </c>
       <c r="E46">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3123,7 +3117,7 @@
         <v>45</v>
       </c>
       <c r="E47">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3132,7 +3126,7 @@
         <v>46</v>
       </c>
       <c r="E48">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3141,7 +3135,7 @@
         <v>47</v>
       </c>
       <c r="E49">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3150,7 +3144,7 @@
         <v>48</v>
       </c>
       <c r="E50">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3159,7 +3153,7 @@
         <v>49</v>
       </c>
       <c r="E51">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3168,7 +3162,7 @@
         <v>50</v>
       </c>
       <c r="E52">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3177,7 +3171,7 @@
         <v>51</v>
       </c>
       <c r="E53">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3186,7 +3180,7 @@
         <v>52</v>
       </c>
       <c r="E54">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3195,7 +3189,7 @@
         <v>53</v>
       </c>
       <c r="E55">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3204,7 +3198,7 @@
         <v>54</v>
       </c>
       <c r="E56">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3213,7 +3207,7 @@
         <v>55</v>
       </c>
       <c r="E57">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3222,7 +3216,7 @@
         <v>56</v>
       </c>
       <c r="E58">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3231,7 +3225,7 @@
         <v>57</v>
       </c>
       <c r="E59">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3240,7 +3234,7 @@
         <v>58</v>
       </c>
       <c r="E60">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3249,7 +3243,7 @@
         <v>59</v>
       </c>
       <c r="E61">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3258,7 +3252,7 @@
         <v>60</v>
       </c>
       <c r="E62">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3267,7 +3261,7 @@
         <v>61</v>
       </c>
       <c r="E63">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3276,7 +3270,7 @@
         <v>62</v>
       </c>
       <c r="E64">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3285,7 +3279,7 @@
         <v>63</v>
       </c>
       <c r="E65">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3294,7 +3288,7 @@
         <v>64</v>
       </c>
       <c r="E66">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3303,7 +3297,7 @@
         <v>65</v>
       </c>
       <c r="E67">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3312,7 +3306,7 @@
         <v>66</v>
       </c>
       <c r="E68">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3321,7 +3315,7 @@
         <v>67</v>
       </c>
       <c r="E69">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3330,7 +3324,7 @@
         <v>68</v>
       </c>
       <c r="E70">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3339,7 +3333,7 @@
         <v>69</v>
       </c>
       <c r="E71">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3348,7 +3342,7 @@
         <v>70</v>
       </c>
       <c r="E72">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3357,7 +3351,7 @@
         <v>71</v>
       </c>
       <c r="E73">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3366,7 +3360,7 @@
         <v>72</v>
       </c>
       <c r="E74">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3375,7 +3369,7 @@
         <v>73</v>
       </c>
       <c r="E75">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3384,7 +3378,7 @@
         <v>74</v>
       </c>
       <c r="E76">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3393,7 +3387,7 @@
         <v>75</v>
       </c>
       <c r="E77">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3402,7 +3396,7 @@
         <v>76</v>
       </c>
       <c r="E78">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3411,7 +3405,7 @@
         <v>77</v>
       </c>
       <c r="E79">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3420,7 +3414,7 @@
         <v>78</v>
       </c>
       <c r="E80">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3429,7 +3423,7 @@
         <v>79</v>
       </c>
       <c r="E81">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3438,7 +3432,7 @@
         <v>80</v>
       </c>
       <c r="E82">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3447,7 +3441,7 @@
         <v>81</v>
       </c>
       <c r="E83">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3456,7 +3450,7 @@
         <v>82</v>
       </c>
       <c r="E84">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3465,7 +3459,7 @@
         <v>83</v>
       </c>
       <c r="E85">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3474,7 +3468,7 @@
         <v>84</v>
       </c>
       <c r="E86">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3483,7 +3477,7 @@
         <v>85</v>
       </c>
       <c r="E87">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3492,7 +3486,7 @@
         <v>86</v>
       </c>
       <c r="E88">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3501,7 +3495,7 @@
         <v>87</v>
       </c>
       <c r="E89">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3510,7 +3504,7 @@
         <v>88</v>
       </c>
       <c r="E90">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3519,7 +3513,7 @@
         <v>89</v>
       </c>
       <c r="E91">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3528,7 +3522,7 @@
         <v>90</v>
       </c>
       <c r="E92">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3537,7 +3531,7 @@
         <v>91</v>
       </c>
       <c r="E93">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3546,7 +3540,7 @@
         <v>92</v>
       </c>
       <c r="E94">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3555,7 +3549,7 @@
         <v>93</v>
       </c>
       <c r="E95">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3564,7 +3558,7 @@
         <v>94</v>
       </c>
       <c r="E96">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3573,7 +3567,7 @@
         <v>95</v>
       </c>
       <c r="E97">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3582,7 +3576,7 @@
         <v>96</v>
       </c>
       <c r="E98">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3591,7 +3585,7 @@
         <v>97</v>
       </c>
       <c r="E99">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3600,7 +3594,7 @@
         <v>98</v>
       </c>
       <c r="E100">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3609,7 +3603,7 @@
         <v>99</v>
       </c>
       <c r="E101">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3618,7 +3612,7 @@
         <v>100</v>
       </c>
       <c r="E102">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3627,7 +3621,7 @@
         <v>101</v>
       </c>
       <c r="E103">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3636,7 +3630,7 @@
         <v>102</v>
       </c>
       <c r="E104">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3645,7 +3639,7 @@
         <v>103</v>
       </c>
       <c r="E105">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3654,7 +3648,7 @@
         <v>104</v>
       </c>
       <c r="E106">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3663,7 +3657,7 @@
         <v>105</v>
       </c>
       <c r="E107">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3672,7 +3666,7 @@
         <v>106</v>
       </c>
       <c r="E108">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3681,7 +3675,7 @@
         <v>107</v>
       </c>
       <c r="E109">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3690,7 +3684,7 @@
         <v>108</v>
       </c>
       <c r="E110">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3699,7 +3693,7 @@
         <v>109</v>
       </c>
       <c r="E111">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3708,7 +3702,7 @@
         <v>110</v>
       </c>
       <c r="E112">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3717,7 +3711,7 @@
         <v>111</v>
       </c>
       <c r="E113">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3726,7 +3720,7 @@
         <v>112</v>
       </c>
       <c r="E114">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3735,7 +3729,7 @@
         <v>113</v>
       </c>
       <c r="E115">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3744,7 +3738,7 @@
         <v>114</v>
       </c>
       <c r="E116">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3753,7 +3747,7 @@
         <v>115</v>
       </c>
       <c r="E117">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3762,7 +3756,7 @@
         <v>116</v>
       </c>
       <c r="E118">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3771,7 +3765,7 @@
         <v>117</v>
       </c>
       <c r="E119">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3780,7 +3774,7 @@
         <v>118</v>
       </c>
       <c r="E120">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3789,7 +3783,7 @@
         <v>119</v>
       </c>
       <c r="E121">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3798,7 +3792,7 @@
         <v>120</v>
       </c>
       <c r="E122">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3807,7 +3801,7 @@
         <v>121</v>
       </c>
       <c r="E123">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3816,7 +3810,7 @@
         <v>122</v>
       </c>
       <c r="E124">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3825,7 +3819,7 @@
         <v>123</v>
       </c>
       <c r="E125">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3834,7 +3828,7 @@
         <v>124</v>
       </c>
       <c r="E126">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3843,7 +3837,7 @@
         <v>125</v>
       </c>
       <c r="E127">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3852,7 +3846,7 @@
         <v>126</v>
       </c>
       <c r="E128">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3861,7 +3855,7 @@
         <v>127</v>
       </c>
       <c r="E129">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3870,7 +3864,7 @@
         <v>128</v>
       </c>
       <c r="E130">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3879,7 +3873,7 @@
         <v>129</v>
       </c>
       <c r="E131">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3888,7 +3882,7 @@
         <v>130</v>
       </c>
       <c r="E132">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3897,7 +3891,7 @@
         <v>131</v>
       </c>
       <c r="E133">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3906,7 +3900,7 @@
         <v>132</v>
       </c>
       <c r="E134">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3915,7 +3909,7 @@
         <v>133</v>
       </c>
       <c r="E135">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3924,7 +3918,7 @@
         <v>134</v>
       </c>
       <c r="E136">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3933,7 +3927,7 @@
         <v>135</v>
       </c>
       <c r="E137">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3942,7 +3936,7 @@
         <v>136</v>
       </c>
       <c r="E138">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3951,7 +3945,7 @@
         <v>137</v>
       </c>
       <c r="E139">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3960,7 +3954,7 @@
         <v>138</v>
       </c>
       <c r="E140">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3969,7 +3963,7 @@
         <v>139</v>
       </c>
       <c r="E141">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3978,7 +3972,7 @@
         <v>140</v>
       </c>
       <c r="E142">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3987,7 +3981,7 @@
         <v>141</v>
       </c>
       <c r="E143">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3996,7 +3990,7 @@
         <v>142</v>
       </c>
       <c r="E144">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4005,7 +3999,7 @@
         <v>143</v>
       </c>
       <c r="E145">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4014,7 +4008,7 @@
         <v>144</v>
       </c>
       <c r="E146">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4023,7 +4017,7 @@
         <v>145</v>
       </c>
       <c r="E147">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4032,7 +4026,7 @@
         <v>146</v>
       </c>
       <c r="E148">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4041,7 +4035,7 @@
         <v>147</v>
       </c>
       <c r="E149">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4050,7 +4044,7 @@
         <v>148</v>
       </c>
       <c r="E150">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4059,7 +4053,7 @@
         <v>149</v>
       </c>
       <c r="E151">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4068,7 +4062,7 @@
         <v>150</v>
       </c>
       <c r="E152">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4077,7 +4071,7 @@
         <v>151</v>
       </c>
       <c r="E153">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4086,7 +4080,7 @@
         <v>152</v>
       </c>
       <c r="E154">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4095,7 +4089,7 @@
         <v>153</v>
       </c>
       <c r="E155">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4104,7 +4098,7 @@
         <v>154</v>
       </c>
       <c r="E156">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4113,7 +4107,7 @@
         <v>155</v>
       </c>
       <c r="E157">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4122,7 +4116,7 @@
         <v>156</v>
       </c>
       <c r="E158">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4131,7 +4125,7 @@
         <v>157</v>
       </c>
       <c r="E159">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4140,7 +4134,7 @@
         <v>158</v>
       </c>
       <c r="E160">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4149,7 +4143,7 @@
         <v>159</v>
       </c>
       <c r="E161">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4158,7 +4152,7 @@
         <v>160</v>
       </c>
       <c r="E162">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4167,7 +4161,7 @@
         <v>161</v>
       </c>
       <c r="E163">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4176,7 +4170,7 @@
         <v>162</v>
       </c>
       <c r="E164">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4185,7 +4179,7 @@
         <v>163</v>
       </c>
       <c r="E165">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4194,7 +4188,7 @@
         <v>164</v>
       </c>
       <c r="E166">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4203,7 +4197,7 @@
         <v>165</v>
       </c>
       <c r="E167">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4212,7 +4206,7 @@
         <v>166</v>
       </c>
       <c r="E168">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4221,7 +4215,7 @@
         <v>167</v>
       </c>
       <c r="E169">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4230,7 +4224,7 @@
         <v>168</v>
       </c>
       <c r="E170">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4239,7 +4233,7 @@
         <v>169</v>
       </c>
       <c r="E171">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4248,7 +4242,7 @@
         <v>170</v>
       </c>
       <c r="E172">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4257,7 +4251,7 @@
         <v>171</v>
       </c>
       <c r="E173">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4266,7 +4260,7 @@
         <v>172</v>
       </c>
       <c r="E174">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4275,7 +4269,7 @@
         <v>173</v>
       </c>
       <c r="E175">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4284,7 +4278,7 @@
         <v>174</v>
       </c>
       <c r="E176">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4293,7 +4287,7 @@
         <v>175</v>
       </c>
       <c r="E177">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4302,7 +4296,7 @@
         <v>176</v>
       </c>
       <c r="E178">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4311,7 +4305,7 @@
         <v>177</v>
       </c>
       <c r="E179">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4320,7 +4314,7 @@
         <v>178</v>
       </c>
       <c r="E180">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4329,7 +4323,7 @@
         <v>179</v>
       </c>
       <c r="E181">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4338,7 +4332,7 @@
         <v>180</v>
       </c>
       <c r="E182">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4347,7 +4341,7 @@
         <v>181</v>
       </c>
       <c r="E183">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4356,7 +4350,7 @@
         <v>182</v>
       </c>
       <c r="E184">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4365,7 +4359,7 @@
         <v>183</v>
       </c>
       <c r="E185">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4374,7 +4368,7 @@
         <v>184</v>
       </c>
       <c r="E186">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4383,7 +4377,7 @@
         <v>185</v>
       </c>
       <c r="E187">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4392,7 +4386,7 @@
         <v>186</v>
       </c>
       <c r="E188">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4401,7 +4395,7 @@
         <v>187</v>
       </c>
       <c r="E189">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4410,7 +4404,7 @@
         <v>188</v>
       </c>
       <c r="E190">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4419,7 +4413,7 @@
         <v>189</v>
       </c>
       <c r="E191">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4428,7 +4422,7 @@
         <v>190</v>
       </c>
       <c r="E192">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4437,7 +4431,7 @@
         <v>191</v>
       </c>
       <c r="E193">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4446,7 +4440,7 @@
         <v>192</v>
       </c>
       <c r="E194">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4455,7 +4449,7 @@
         <v>193</v>
       </c>
       <c r="E195">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4464,7 +4458,7 @@
         <v>194</v>
       </c>
       <c r="E196">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4473,7 +4467,7 @@
         <v>195</v>
       </c>
       <c r="E197">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4482,7 +4476,7 @@
         <v>196</v>
       </c>
       <c r="E198">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4491,7 +4485,7 @@
         <v>197</v>
       </c>
       <c r="E199">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4500,7 +4494,7 @@
         <v>198</v>
       </c>
       <c r="E200">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4509,7 +4503,7 @@
         <v>199</v>
       </c>
       <c r="E201">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4518,7 +4512,7 @@
         <v>200</v>
       </c>
       <c r="E202">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4527,7 +4521,7 @@
         <v>201</v>
       </c>
       <c r="E203">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4536,7 +4530,7 @@
         <v>202</v>
       </c>
       <c r="E204">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4545,7 +4539,7 @@
         <v>203</v>
       </c>
       <c r="E205">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4554,7 +4548,7 @@
         <v>204</v>
       </c>
       <c r="E206">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4563,7 +4557,7 @@
         <v>205</v>
       </c>
       <c r="E207">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4572,7 +4566,7 @@
         <v>206</v>
       </c>
       <c r="E208">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4581,7 +4575,7 @@
         <v>207</v>
       </c>
       <c r="E209">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4590,7 +4584,7 @@
         <v>208</v>
       </c>
       <c r="E210">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4599,7 +4593,7 @@
         <v>209</v>
       </c>
       <c r="E211">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4608,7 +4602,7 @@
         <v>210</v>
       </c>
       <c r="E212">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4617,7 +4611,7 @@
         <v>211</v>
       </c>
       <c r="E213">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4626,7 +4620,7 @@
         <v>212</v>
       </c>
       <c r="E214">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4635,7 +4629,7 @@
         <v>213</v>
       </c>
       <c r="E215">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4644,7 +4638,7 @@
         <v>214</v>
       </c>
       <c r="E216">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4653,7 +4647,7 @@
         <v>215</v>
       </c>
       <c r="E217">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4662,7 +4656,7 @@
         <v>216</v>
       </c>
       <c r="E218">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4671,7 +4665,7 @@
         <v>217</v>
       </c>
       <c r="E219">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4680,7 +4674,7 @@
         <v>218</v>
       </c>
       <c r="E220">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4689,7 +4683,7 @@
         <v>219</v>
       </c>
       <c r="E221">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4698,7 +4692,7 @@
         <v>220</v>
       </c>
       <c r="E222">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4707,7 +4701,7 @@
         <v>221</v>
       </c>
       <c r="E223">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4716,7 +4710,7 @@
         <v>222</v>
       </c>
       <c r="E224">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4725,7 +4719,7 @@
         <v>223</v>
       </c>
       <c r="E225">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4734,7 +4728,7 @@
         <v>224</v>
       </c>
       <c r="E226">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4743,7 +4737,7 @@
         <v>225</v>
       </c>
       <c r="E227">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4752,7 +4746,7 @@
         <v>226</v>
       </c>
       <c r="E228">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4761,7 +4755,7 @@
         <v>227</v>
       </c>
       <c r="E229">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4770,7 +4764,7 @@
         <v>228</v>
       </c>
       <c r="E230">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4779,7 +4773,7 @@
         <v>229</v>
       </c>
       <c r="E231">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4788,7 +4782,7 @@
         <v>230</v>
       </c>
       <c r="E232">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4797,7 +4791,7 @@
         <v>231</v>
       </c>
       <c r="E233">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4806,7 +4800,7 @@
         <v>232</v>
       </c>
       <c r="E234">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4815,7 +4809,7 @@
         <v>233</v>
       </c>
       <c r="E235">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4824,7 +4818,7 @@
         <v>234</v>
       </c>
       <c r="E236">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4833,7 +4827,7 @@
         <v>235</v>
       </c>
       <c r="E237">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4842,7 +4836,7 @@
         <v>236</v>
       </c>
       <c r="E238">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4851,7 +4845,7 @@
         <v>237</v>
       </c>
       <c r="E239">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4860,7 +4854,7 @@
         <v>238</v>
       </c>
       <c r="E240">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4869,7 +4863,7 @@
         <v>239</v>
       </c>
       <c r="E241">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4878,7 +4872,7 @@
         <v>240</v>
       </c>
       <c r="E242">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4887,7 +4881,7 @@
         <v>241</v>
       </c>
       <c r="E243">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4896,7 +4890,7 @@
         <v>242</v>
       </c>
       <c r="E244">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4905,7 +4899,7 @@
         <v>243</v>
       </c>
       <c r="E245">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4914,7 +4908,7 @@
         <v>244</v>
       </c>
       <c r="E246">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4923,7 +4917,7 @@
         <v>245</v>
       </c>
       <c r="E247">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4932,7 +4926,7 @@
         <v>246</v>
       </c>
       <c r="E248">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4941,7 +4935,7 @@
         <v>247</v>
       </c>
       <c r="E249">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4950,7 +4944,7 @@
         <v>248</v>
       </c>
       <c r="E250">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4959,7 +4953,7 @@
         <v>249</v>
       </c>
       <c r="E251">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4968,7 +4962,7 @@
         <v>250</v>
       </c>
       <c r="E252">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4977,7 +4971,7 @@
         <v>251</v>
       </c>
       <c r="E253">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4986,7 +4980,7 @@
         <v>252</v>
       </c>
       <c r="E254">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4995,7 +4989,7 @@
         <v>253</v>
       </c>
       <c r="E255">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5004,7 +4998,7 @@
         <v>254</v>
       </c>
       <c r="E256">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5013,7 +5007,7 @@
         <v>255</v>
       </c>
       <c r="E257">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5022,7 +5016,7 @@
         <v>256</v>
       </c>
       <c r="E258">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5031,7 +5025,7 @@
         <v>257</v>
       </c>
       <c r="E259">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5040,7 +5034,7 @@
         <v>258</v>
       </c>
       <c r="E260">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5049,7 +5043,7 @@
         <v>259</v>
       </c>
       <c r="E261">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5058,7 +5052,7 @@
         <v>260</v>
       </c>
       <c r="E262">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5067,7 +5061,7 @@
         <v>261</v>
       </c>
       <c r="E263">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5076,7 +5070,7 @@
         <v>262</v>
       </c>
       <c r="E264">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5085,7 +5079,7 @@
         <v>263</v>
       </c>
       <c r="E265">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5094,7 +5088,7 @@
         <v>264</v>
       </c>
       <c r="E266">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5103,7 +5097,7 @@
         <v>265</v>
       </c>
       <c r="E267">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5112,7 +5106,7 @@
         <v>266</v>
       </c>
       <c r="E268">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5121,7 +5115,7 @@
         <v>267</v>
       </c>
       <c r="E269">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5130,7 +5124,7 @@
         <v>268</v>
       </c>
       <c r="E270">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5139,7 +5133,7 @@
         <v>269</v>
       </c>
       <c r="E271">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5148,7 +5142,7 @@
         <v>270</v>
       </c>
       <c r="E272">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5157,7 +5151,7 @@
         <v>271</v>
       </c>
       <c r="E273">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5166,7 +5160,7 @@
         <v>272</v>
       </c>
       <c r="E274">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5175,7 +5169,7 @@
         <v>273</v>
       </c>
       <c r="E275">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5184,7 +5178,7 @@
         <v>274</v>
       </c>
       <c r="E276">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5193,7 +5187,7 @@
         <v>275</v>
       </c>
       <c r="E277">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5202,7 +5196,7 @@
         <v>276</v>
       </c>
       <c r="E278">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5211,7 +5205,7 @@
         <v>277</v>
       </c>
       <c r="E279">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5220,7 +5214,7 @@
         <v>278</v>
       </c>
       <c r="E280">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5229,7 +5223,7 @@
         <v>279</v>
       </c>
       <c r="E281">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5238,7 +5232,7 @@
         <v>280</v>
       </c>
       <c r="E282">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5247,7 +5241,7 @@
         <v>281</v>
       </c>
       <c r="E283">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5256,7 +5250,7 @@
         <v>282</v>
       </c>
       <c r="E284">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5265,7 +5259,7 @@
         <v>283</v>
       </c>
       <c r="E285">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5274,7 +5268,7 @@
         <v>284</v>
       </c>
       <c r="E286">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5283,7 +5277,7 @@
         <v>285</v>
       </c>
       <c r="E287">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5292,7 +5286,7 @@
         <v>286</v>
       </c>
       <c r="E288">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5301,7 +5295,7 @@
         <v>287</v>
       </c>
       <c r="E289">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5310,7 +5304,7 @@
         <v>288</v>
       </c>
       <c r="E290">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5319,7 +5313,7 @@
         <v>289</v>
       </c>
       <c r="E291">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5328,7 +5322,7 @@
         <v>290</v>
       </c>
       <c r="E292">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5337,7 +5331,7 @@
         <v>291</v>
       </c>
       <c r="E293">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5346,7 +5340,7 @@
         <v>292</v>
       </c>
       <c r="E294">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5355,7 +5349,7 @@
         <v>293</v>
       </c>
       <c r="E295">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5364,7 +5358,7 @@
         <v>294</v>
       </c>
       <c r="E296">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5373,7 +5367,7 @@
         <v>295</v>
       </c>
       <c r="E297">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5382,7 +5376,7 @@
         <v>296</v>
       </c>
       <c r="E298">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5391,7 +5385,7 @@
         <v>297</v>
       </c>
       <c r="E299">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5400,7 +5394,7 @@
         <v>298</v>
       </c>
       <c r="E300">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5409,7 +5403,7 @@
         <v>299</v>
       </c>
       <c r="E301">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5418,7 +5412,7 @@
         <v>300</v>
       </c>
       <c r="E302">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5427,7 +5421,7 @@
         <v>301</v>
       </c>
       <c r="E303">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5436,7 +5430,7 @@
         <v>302</v>
       </c>
       <c r="E304">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5445,7 +5439,7 @@
         <v>303</v>
       </c>
       <c r="E305">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5454,7 +5448,7 @@
         <v>304</v>
       </c>
       <c r="E306">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5463,7 +5457,7 @@
         <v>305</v>
       </c>
       <c r="E307">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5472,7 +5466,7 @@
         <v>306</v>
       </c>
       <c r="E308">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5481,7 +5475,7 @@
         <v>307</v>
       </c>
       <c r="E309">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5490,7 +5484,7 @@
         <v>308</v>
       </c>
       <c r="E310">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5499,7 +5493,7 @@
         <v>309</v>
       </c>
       <c r="E311">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5508,7 +5502,7 @@
         <v>310</v>
       </c>
       <c r="E312">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5517,7 +5511,7 @@
         <v>311</v>
       </c>
       <c r="E313">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5526,7 +5520,7 @@
         <v>312</v>
       </c>
       <c r="E314">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5535,7 +5529,7 @@
         <v>313</v>
       </c>
       <c r="E315">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5544,7 +5538,7 @@
         <v>314</v>
       </c>
       <c r="E316">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5553,7 +5547,7 @@
         <v>315</v>
       </c>
       <c r="E317">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5562,7 +5556,7 @@
         <v>316</v>
       </c>
       <c r="E318">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5571,7 +5565,7 @@
         <v>317</v>
       </c>
       <c r="E319">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5580,7 +5574,7 @@
         <v>318</v>
       </c>
       <c r="E320">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5589,7 +5583,7 @@
         <v>319</v>
       </c>
       <c r="E321">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5598,7 +5592,7 @@
         <v>320</v>
       </c>
       <c r="E322">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5607,7 +5601,7 @@
         <v>321</v>
       </c>
       <c r="E323">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5616,7 +5610,7 @@
         <v>322</v>
       </c>
       <c r="E324">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5625,7 +5619,7 @@
         <v>323</v>
       </c>
       <c r="E325">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5634,7 +5628,7 @@
         <v>324</v>
       </c>
       <c r="E326">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5643,7 +5637,7 @@
         <v>325</v>
       </c>
       <c r="E327">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5652,7 +5646,7 @@
         <v>326</v>
       </c>
       <c r="E328">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5661,7 +5655,7 @@
         <v>327</v>
       </c>
       <c r="E329">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5670,7 +5664,7 @@
         <v>328</v>
       </c>
       <c r="E330">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5679,7 +5673,7 @@
         <v>329</v>
       </c>
       <c r="E331">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5688,7 +5682,7 @@
         <v>330</v>
       </c>
       <c r="E332">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5697,7 +5691,7 @@
         <v>331</v>
       </c>
       <c r="E333">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5706,7 +5700,7 @@
         <v>332</v>
       </c>
       <c r="E334">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5715,7 +5709,7 @@
         <v>333</v>
       </c>
       <c r="E335">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5724,7 +5718,7 @@
         <v>334</v>
       </c>
       <c r="E336">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5733,7 +5727,7 @@
         <v>335</v>
       </c>
       <c r="E337">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5742,7 +5736,7 @@
         <v>336</v>
       </c>
       <c r="E338">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5751,7 +5745,7 @@
         <v>337</v>
       </c>
       <c r="E339">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5760,7 +5754,7 @@
         <v>338</v>
       </c>
       <c r="E340">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5769,7 +5763,7 @@
         <v>339</v>
       </c>
       <c r="E341">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5778,7 +5772,7 @@
         <v>340</v>
       </c>
       <c r="E342">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5787,7 +5781,7 @@
         <v>341</v>
       </c>
       <c r="E343">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5796,7 +5790,7 @@
         <v>342</v>
       </c>
       <c r="E344">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5805,7 +5799,7 @@
         <v>343</v>
       </c>
       <c r="E345">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5814,7 +5808,7 @@
         <v>344</v>
       </c>
       <c r="E346">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5823,7 +5817,7 @@
         <v>345</v>
       </c>
       <c r="E347">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5832,7 +5826,7 @@
         <v>346</v>
       </c>
       <c r="E348">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5841,7 +5835,7 @@
         <v>347</v>
       </c>
       <c r="E349">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5850,7 +5844,7 @@
         <v>348</v>
       </c>
       <c r="E350">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5859,7 +5853,7 @@
         <v>349</v>
       </c>
       <c r="E351">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5868,7 +5862,7 @@
         <v>350</v>
       </c>
       <c r="E352">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5877,7 +5871,7 @@
         <v>351</v>
       </c>
       <c r="E353">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5886,7 +5880,7 @@
         <v>352</v>
       </c>
       <c r="E354">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5895,7 +5889,7 @@
         <v>353</v>
       </c>
       <c r="E355">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5904,7 +5898,7 @@
         <v>354</v>
       </c>
       <c r="E356">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5913,7 +5907,7 @@
         <v>355</v>
       </c>
       <c r="E357">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5922,7 +5916,7 @@
         <v>356</v>
       </c>
       <c r="E358">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5931,7 +5925,7 @@
         <v>357</v>
       </c>
       <c r="E359">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5940,7 +5934,7 @@
         <v>358</v>
       </c>
       <c r="E360">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5949,7 +5943,7 @@
         <v>359</v>
       </c>
       <c r="E361">
-        <f>IF(ABS(ABS(ROW()-Sheet1!C3-2-180)-180)&lt;10,8-(0.25*ABS(ABS(ROW()-Sheet1!C3-2-180)-180)),0)</f>
+        <f>IF(ABS(ABS(ROW()-Sheet1!A3-2-180)-180)&lt;15,8-(0.4*ABS(ABS(ROW()-Sheet1!A3-2-180)-180)),0)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove unnecessary B line
</commit_message>
<xml_diff>
--- a/hello.xlsx
+++ b/hello.xlsx
@@ -15,15 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Chart Title</t>
   </si>
   <si>
     <t>Dial Colors</t>
-  </si>
-  <si>
-    <t>Needle</t>
   </si>
 </sst>
 </file>
@@ -2671,17 +2668,11 @@
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
         <v>60</v>
       </c>
-      <c r="B2">
-        <v>180</v>
-      </c>
       <c r="D2">
         <v>0</v>
       </c>
@@ -2694,10 +2685,6 @@
       <c r="A3">
         <v>60</v>
       </c>
-      <c r="B3">
-        <f>((180/200)*(Sheet1!A3+100))-B4</f>
-        <v>0</v>
-      </c>
       <c r="D3">
         <v>1</v>
       </c>
@@ -2710,9 +2697,6 @@
       <c r="A4">
         <v>60</v>
       </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
       <c r="D4">
         <v>2</v>
       </c>
@@ -2724,10 +2708,6 @@
     <row r="5" spans="1:5">
       <c r="A5">
         <v>60</v>
-      </c>
-      <c r="B5">
-        <f>360-SUM(B2:B4)</f>
-        <v>0</v>
       </c>
       <c r="D5">
         <v>3</v>

</xml_diff>